<commit_message>
Format and clean code retrieve futur load
</commit_message>
<xml_diff>
--- a/scenario_builder_tool_input.xlsx
+++ b/scenario_builder_tool_input.xlsx
@@ -5,19 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/climact/patex-container/dev/_common/scenario_builder/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/climact/pypsa/pypsa-eur-climact/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230054EB-21BA-4B49-88EC-526F1EC14CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6CDC03-F068-1C41-B1E8-5B71FE0F0E04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Levers" sheetId="1" r:id="rId1"/>
-    <sheet name="Variables" sheetId="14" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Variables!$A$1:$A$19</definedName>
     <definedName name="variable_list">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -38,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="245">
   <si>
     <t>country / scenario</t>
   </si>
@@ -755,9 +753,6 @@
     <t>Fossil fuels</t>
   </si>
   <si>
-    <t>metrics</t>
-  </si>
-  <si>
     <t>Water</t>
   </si>
   <si>
@@ -777,60 +772,6 @@
   </si>
   <si>
     <t>Scenario</t>
-  </si>
-  <si>
-    <t>tra_energy-demand_domestic_electricity_BEV_passenger_2W[TWh]</t>
-  </si>
-  <si>
-    <t>tra_energy-demand_domestic_electricity_BEV_freight_HDV[TWh]</t>
-  </si>
-  <si>
-    <t>tra_energy-demand_domestic_electricity_PHEV_freight_HDV[TWh]</t>
-  </si>
-  <si>
-    <t>tra_energy-demand_domestic_electricity_PHEVCE_freight_HDV[TWh]</t>
-  </si>
-  <si>
-    <t>tra_energy-demand_domestic_electricity_BEV_freight_IWW[TWh]</t>
-  </si>
-  <si>
-    <t>tra_energy-demand_domestic_electricity_BEV_freight_LDV[TWh]</t>
-  </si>
-  <si>
-    <t>tra_energy-demand_domestic_electricity_PHEV_freight_LDV[TWh]</t>
-  </si>
-  <si>
-    <t>tra_energy-demand_domestic_electricity_BEV_passenger_LDV[TWh]</t>
-  </si>
-  <si>
-    <t>tra_energy-demand_domestic_electricity_PHEV_passenger_LDV[TWh]</t>
-  </si>
-  <si>
-    <t>tra_energy-demand_bunkers-aviation_electricity_BEV_freight_aviation[TWh]</t>
-  </si>
-  <si>
-    <t>tra_energy-demand_domestic_electricity_BEV_freight_aviation[TWh]</t>
-  </si>
-  <si>
-    <t>tra_energy-demand_bunkers-aviation_electricity_BEV_passenger_aviation[TWh]</t>
-  </si>
-  <si>
-    <t>tra_energy-demand_domestic_electricity_BEV_passenger_aviation[TWh]</t>
-  </si>
-  <si>
-    <t>tra_energy-demand_domestic_electricity_BEV_passenger_bus[TWh]</t>
-  </si>
-  <si>
-    <t>tra_energy-demand_domestic_electricity_PHEV_passenger_bus[TWh]</t>
-  </si>
-  <si>
-    <t>tra_energy-demand_bunkers-marine_electricity_BEV_freight_marine[TWh]</t>
-  </si>
-  <si>
-    <t>tra_energy-demand_domestic_electricity_CEV_freight_rail[TWh]</t>
-  </si>
-  <si>
-    <t>tra_energy-demand_domestic_electricity_CEV_passenger_rail[TWh]</t>
   </si>
 </sst>
 </file>
@@ -895,9 +836,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
@@ -914,25 +854,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1008,19 +930,19 @@
   </dxfs>
   <tableStyles count="3">
     <tableStyle name="Levers-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="headerRow" dxfId="9"/>
-      <tableStyleElement type="firstRowStripe" dxfId="8"/>
-      <tableStyleElement type="secondRowStripe" dxfId="7"/>
+      <tableStyleElement type="headerRow" dxfId="8"/>
+      <tableStyleElement type="firstRowStripe" dxfId="7"/>
+      <tableStyleElement type="secondRowStripe" dxfId="6"/>
     </tableStyle>
     <tableStyle name="Levers-style 2" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="headerRow" dxfId="6"/>
-      <tableStyleElement type="firstRowStripe" dxfId="5"/>
-      <tableStyleElement type="secondRowStripe" dxfId="4"/>
+      <tableStyleElement type="headerRow" dxfId="5"/>
+      <tableStyleElement type="firstRowStripe" dxfId="4"/>
+      <tableStyleElement type="secondRowStripe" dxfId="3"/>
     </tableStyle>
     <tableStyle name="Levers-style 3" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}">
-      <tableStyleElement type="headerRow" dxfId="3"/>
-      <tableStyleElement type="firstRowStripe" dxfId="2"/>
-      <tableStyleElement type="secondRowStripe" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="secondRowStripe" dxfId="0"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1032,16 +954,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A5780B96-78DC-5240-86CE-F0B05EAEF3C6}" name="Table2" displayName="Table2" ref="A1:A19" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:A19" xr:uid="{A5780B96-78DC-5240-86CE-F0B05EAEF3C6}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{36F5D792-D9C4-B549-B165-2DE85CB5AFF4}" name="metrics"/>
-  </tableColumns>
-  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1347,7 +1259,7 @@
   </sheetPr>
   <dimension ref="A1:AE220"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="AE187" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -1364,14 +1276,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="13" x14ac:dyDescent="0.15">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
       <c r="E1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
@@ -1453,111 +1365,111 @@
       </c>
     </row>
     <row r="2" spans="1:31" ht="216.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>245</v>
+      <c r="E2" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="3" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E3">
@@ -1643,16 +1555,16 @@
       </c>
     </row>
     <row r="4" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E4">
@@ -1738,16 +1650,16 @@
       </c>
     </row>
     <row r="5" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E5">
@@ -1833,16 +1745,16 @@
       </c>
     </row>
     <row r="6" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>38</v>
       </c>
       <c r="E6">
@@ -1928,16 +1840,16 @@
       </c>
     </row>
     <row r="7" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E7">
@@ -2023,16 +1935,16 @@
       </c>
     </row>
     <row r="8" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>41</v>
       </c>
       <c r="E8">
@@ -2118,16 +2030,16 @@
       </c>
     </row>
     <row r="9" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E9">
@@ -2213,16 +2125,16 @@
       </c>
     </row>
     <row r="10" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>41</v>
       </c>
       <c r="E10">
@@ -2308,16 +2220,16 @@
       </c>
     </row>
     <row r="11" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>44</v>
       </c>
       <c r="E11">
@@ -2403,16 +2315,16 @@
       </c>
     </row>
     <row r="12" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>47</v>
       </c>
       <c r="E12">
@@ -2498,16 +2410,16 @@
       </c>
     </row>
     <row r="13" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>48</v>
       </c>
       <c r="E13">
@@ -2593,16 +2505,16 @@
       </c>
     </row>
     <row r="14" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>49</v>
       </c>
       <c r="E14">
@@ -2688,16 +2600,16 @@
       </c>
     </row>
     <row r="15" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>50</v>
       </c>
       <c r="E15">
@@ -2783,16 +2695,16 @@
       </c>
     </row>
     <row r="16" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E16">
@@ -2878,16 +2790,16 @@
       </c>
     </row>
     <row r="17" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="3" t="s">
         <v>53</v>
       </c>
       <c r="E17">
@@ -2973,16 +2885,16 @@
       </c>
     </row>
     <row r="18" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="3" t="s">
         <v>54</v>
       </c>
       <c r="E18">
@@ -3068,16 +2980,16 @@
       </c>
     </row>
     <row r="19" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="3" t="s">
         <v>55</v>
       </c>
       <c r="E19">
@@ -3163,16 +3075,16 @@
       </c>
     </row>
     <row r="20" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="3" t="s">
         <v>56</v>
       </c>
       <c r="E20">
@@ -3258,16 +3170,16 @@
       </c>
     </row>
     <row r="21" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="3" t="s">
         <v>57</v>
       </c>
       <c r="E21">
@@ -3353,16 +3265,16 @@
       </c>
     </row>
     <row r="22" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="3" t="s">
         <v>59</v>
       </c>
       <c r="E22">
@@ -3448,14 +3360,14 @@
       </c>
     </row>
     <row r="23" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4" t="s">
+      <c r="C23" s="3"/>
+      <c r="D23" s="3" t="s">
         <v>60</v>
       </c>
       <c r="E23">
@@ -3541,16 +3453,16 @@
       </c>
     </row>
     <row r="24" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="3" t="s">
         <v>59</v>
       </c>
       <c r="E24">
@@ -3636,14 +3548,14 @@
       </c>
     </row>
     <row r="25" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4" t="s">
+      <c r="C25" s="3"/>
+      <c r="D25" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E25">
@@ -3729,16 +3641,16 @@
       </c>
     </row>
     <row r="26" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="3" t="s">
         <v>47</v>
       </c>
       <c r="E26">
@@ -3824,16 +3736,16 @@
       </c>
     </row>
     <row r="27" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="3" t="s">
         <v>48</v>
       </c>
       <c r="E27">
@@ -3919,16 +3831,16 @@
       </c>
     </row>
     <row r="28" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="3" t="s">
         <v>49</v>
       </c>
       <c r="E28">
@@ -4014,16 +3926,16 @@
       </c>
     </row>
     <row r="29" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="3" t="s">
         <v>50</v>
       </c>
       <c r="E29">
@@ -4109,16 +4021,16 @@
       </c>
     </row>
     <row r="30" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E30">
@@ -4204,14 +4116,14 @@
       </c>
     </row>
     <row r="31" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4" t="s">
+      <c r="C31" s="3"/>
+      <c r="D31" s="3" t="s">
         <v>60</v>
       </c>
       <c r="E31">
@@ -4297,14 +4209,14 @@
       </c>
     </row>
     <row r="32" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4" t="s">
+      <c r="C32" s="3"/>
+      <c r="D32" s="3" t="s">
         <v>64</v>
       </c>
       <c r="E32">
@@ -4390,14 +4302,14 @@
       </c>
     </row>
     <row r="33" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4" t="s">
+      <c r="C33" s="3"/>
+      <c r="D33" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E33">
@@ -4483,16 +4395,16 @@
       </c>
     </row>
     <row r="34" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="3" t="s">
         <v>54</v>
       </c>
       <c r="E34">
@@ -4578,16 +4490,16 @@
       </c>
     </row>
     <row r="35" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="3" t="s">
         <v>55</v>
       </c>
       <c r="E35">
@@ -4673,16 +4585,16 @@
       </c>
     </row>
     <row r="36" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D36" s="3" t="s">
         <v>56</v>
       </c>
       <c r="E36">
@@ -4768,16 +4680,16 @@
       </c>
     </row>
     <row r="37" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D37" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E37">
@@ -4863,16 +4775,16 @@
       </c>
     </row>
     <row r="38" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" s="3" t="s">
         <v>70</v>
       </c>
       <c r="E38">
@@ -4958,16 +4870,16 @@
       </c>
     </row>
     <row r="39" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D39" s="3" t="s">
         <v>71</v>
       </c>
       <c r="E39">
@@ -5053,16 +4965,16 @@
       </c>
     </row>
     <row r="40" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D40" s="3" t="s">
         <v>72</v>
       </c>
       <c r="E40">
@@ -5148,16 +5060,16 @@
       </c>
     </row>
     <row r="41" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D41" s="3" t="s">
         <v>74</v>
       </c>
       <c r="E41">
@@ -5243,16 +5155,16 @@
       </c>
     </row>
     <row r="42" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D42" s="3" t="s">
         <v>75</v>
       </c>
       <c r="E42">
@@ -5338,16 +5250,16 @@
       </c>
     </row>
     <row r="43" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D43" s="3" t="s">
         <v>77</v>
       </c>
       <c r="E43">
@@ -5433,16 +5345,16 @@
       </c>
     </row>
     <row r="44" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C44" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D44" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E44">
@@ -5528,16 +5440,16 @@
       </c>
     </row>
     <row r="45" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A45" s="4" t="s">
+      <c r="A45" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C45" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D45" s="3" t="s">
         <v>82</v>
       </c>
       <c r="E45">
@@ -5623,14 +5535,14 @@
       </c>
     </row>
     <row r="46" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4" t="s">
+      <c r="C46" s="3"/>
+      <c r="D46" s="3" t="s">
         <v>83</v>
       </c>
       <c r="E46">
@@ -5716,14 +5628,14 @@
       </c>
     </row>
     <row r="47" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4" t="s">
+      <c r="C47" s="3"/>
+      <c r="D47" s="3" t="s">
         <v>84</v>
       </c>
       <c r="E47">
@@ -5809,14 +5721,14 @@
       </c>
     </row>
     <row r="48" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A48" s="4" t="s">
+      <c r="A48" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4" t="s">
+      <c r="C48" s="3"/>
+      <c r="D48" s="3" t="s">
         <v>85</v>
       </c>
       <c r="E48">
@@ -5902,14 +5814,14 @@
       </c>
     </row>
     <row r="49" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A49" s="4" t="s">
+      <c r="A49" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4" t="s">
+      <c r="C49" s="3"/>
+      <c r="D49" s="3" t="s">
         <v>86</v>
       </c>
       <c r="E49">
@@ -5995,14 +5907,14 @@
       </c>
     </row>
     <row r="50" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A50" s="4" t="s">
+      <c r="A50" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C50" s="4"/>
-      <c r="D50" s="4" t="s">
+      <c r="C50" s="3"/>
+      <c r="D50" s="3" t="s">
         <v>88</v>
       </c>
       <c r="E50">
@@ -6088,16 +6000,16 @@
       </c>
     </row>
     <row r="51" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C51" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="D51" s="3" t="s">
         <v>90</v>
       </c>
       <c r="E51">
@@ -6183,16 +6095,16 @@
       </c>
     </row>
     <row r="52" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A52" s="4" t="s">
+      <c r="A52" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C52" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="D52" s="3" t="s">
         <v>91</v>
       </c>
       <c r="E52">
@@ -6278,16 +6190,16 @@
       </c>
     </row>
     <row r="53" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A53" s="4" t="s">
+      <c r="A53" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C53" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D53" s="4" t="s">
+      <c r="D53" s="3" t="s">
         <v>92</v>
       </c>
       <c r="E53">
@@ -6373,16 +6285,16 @@
       </c>
     </row>
     <row r="54" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A54" s="4" t="s">
+      <c r="A54" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C54" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D54" s="4" t="s">
+      <c r="D54" s="3" t="s">
         <v>93</v>
       </c>
       <c r="E54">
@@ -6468,16 +6380,16 @@
       </c>
     </row>
     <row r="55" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A55" s="4" t="s">
+      <c r="A55" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C55" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D55" s="4" t="s">
+      <c r="D55" s="3" t="s">
         <v>94</v>
       </c>
       <c r="E55">
@@ -6563,14 +6475,14 @@
       </c>
     </row>
     <row r="56" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A56" s="4" t="s">
+      <c r="A56" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C56" s="4"/>
-      <c r="D56" s="4" t="s">
+      <c r="C56" s="3"/>
+      <c r="D56" s="3" t="s">
         <v>95</v>
       </c>
       <c r="E56">
@@ -6656,16 +6568,16 @@
       </c>
     </row>
     <row r="57" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="4" t="s">
+      <c r="A57" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C57" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D57" s="4" t="s">
+      <c r="D57" s="3" t="s">
         <v>97</v>
       </c>
       <c r="E57">
@@ -6751,16 +6663,16 @@
       </c>
     </row>
     <row r="58" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="4" t="s">
+      <c r="A58" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="C58" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D58" s="4" t="s">
+      <c r="D58" s="3" t="s">
         <v>98</v>
       </c>
       <c r="E58">
@@ -6846,14 +6758,14 @@
       </c>
     </row>
     <row r="59" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A59" s="4" t="s">
+      <c r="A59" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C59" s="4"/>
-      <c r="D59" s="4" t="s">
+      <c r="C59" s="3"/>
+      <c r="D59" s="3" t="s">
         <v>88</v>
       </c>
       <c r="E59">
@@ -6939,16 +6851,16 @@
       </c>
     </row>
     <row r="60" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A60" s="4" t="s">
+      <c r="A60" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C60" s="4" t="s">
+      <c r="C60" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D60" s="4" t="s">
+      <c r="D60" s="3" t="s">
         <v>90</v>
       </c>
       <c r="E60">
@@ -7034,16 +6946,16 @@
       </c>
     </row>
     <row r="61" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A61" s="4" t="s">
+      <c r="A61" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="C61" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D61" s="4" t="s">
+      <c r="D61" s="3" t="s">
         <v>91</v>
       </c>
       <c r="E61">
@@ -7129,16 +7041,16 @@
       </c>
     </row>
     <row r="62" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A62" s="4" t="s">
+      <c r="A62" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="C62" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D62" s="4" t="s">
+      <c r="D62" s="3" t="s">
         <v>92</v>
       </c>
       <c r="E62">
@@ -7224,16 +7136,16 @@
       </c>
     </row>
     <row r="63" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A63" s="4" t="s">
+      <c r="A63" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C63" s="4" t="s">
+      <c r="C63" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D63" s="4" t="s">
+      <c r="D63" s="3" t="s">
         <v>93</v>
       </c>
       <c r="E63">
@@ -7319,16 +7231,16 @@
       </c>
     </row>
     <row r="64" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A64" s="4" t="s">
+      <c r="A64" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C64" s="4" t="s">
+      <c r="C64" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D64" s="4" t="s">
+      <c r="D64" s="3" t="s">
         <v>94</v>
       </c>
       <c r="E64">
@@ -7414,14 +7326,14 @@
       </c>
     </row>
     <row r="65" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A65" s="4" t="s">
+      <c r="A65" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B65" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C65" s="4"/>
-      <c r="D65" s="4" t="s">
+      <c r="C65" s="3"/>
+      <c r="D65" s="3" t="s">
         <v>101</v>
       </c>
       <c r="E65">
@@ -7507,14 +7419,14 @@
       </c>
     </row>
     <row r="66" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A66" s="4" t="s">
+      <c r="A66" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B66" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C66" s="4"/>
-      <c r="D66" s="4" t="s">
+      <c r="C66" s="3"/>
+      <c r="D66" s="3" t="s">
         <v>103</v>
       </c>
       <c r="E66">
@@ -7600,16 +7512,16 @@
       </c>
     </row>
     <row r="67" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A67" s="4" t="s">
+      <c r="A67" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B67" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C67" s="4" t="s">
+      <c r="C67" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D67" s="4" t="s">
+      <c r="D67" s="3" t="s">
         <v>105</v>
       </c>
       <c r="E67">
@@ -7695,16 +7607,16 @@
       </c>
     </row>
     <row r="68" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A68" s="4" t="s">
+      <c r="A68" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B68" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C68" s="4" t="s">
+      <c r="C68" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D68" s="4" t="s">
+      <c r="D68" s="3" t="s">
         <v>106</v>
       </c>
       <c r="E68">
@@ -7790,16 +7702,16 @@
       </c>
     </row>
     <row r="69" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A69" s="4" t="s">
+      <c r="A69" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B69" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C69" s="4" t="s">
+      <c r="C69" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D69" s="4" t="s">
+      <c r="D69" s="3" t="s">
         <v>107</v>
       </c>
       <c r="E69">
@@ -7885,16 +7797,16 @@
       </c>
     </row>
     <row r="70" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A70" s="4" t="s">
+      <c r="A70" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B70" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C70" s="4" t="s">
+      <c r="C70" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D70" s="4" t="s">
+      <c r="D70" s="3" t="s">
         <v>105</v>
       </c>
       <c r="E70">
@@ -7980,16 +7892,16 @@
       </c>
     </row>
     <row r="71" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A71" s="4" t="s">
+      <c r="A71" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B71" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C71" s="4" t="s">
+      <c r="C71" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D71" s="4" t="s">
+      <c r="D71" s="3" t="s">
         <v>106</v>
       </c>
       <c r="E71">
@@ -8075,16 +7987,16 @@
       </c>
     </row>
     <row r="72" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A72" s="4" t="s">
+      <c r="A72" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B72" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C72" s="4" t="s">
+      <c r="C72" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D72" s="4" t="s">
+      <c r="D72" s="3" t="s">
         <v>109</v>
       </c>
       <c r="E72">
@@ -8170,16 +8082,16 @@
       </c>
     </row>
     <row r="73" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A73" s="4" t="s">
+      <c r="A73" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B73" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C73" s="4" t="s">
+      <c r="C73" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D73" s="4" t="s">
+      <c r="D73" s="3" t="s">
         <v>107</v>
       </c>
       <c r="E73">
@@ -8265,14 +8177,14 @@
       </c>
     </row>
     <row r="74" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A74" s="4" t="s">
+      <c r="A74" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B74" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C74" s="4"/>
-      <c r="D74" s="4" t="s">
+      <c r="C74" s="3"/>
+      <c r="D74" s="3" t="s">
         <v>112</v>
       </c>
       <c r="E74">
@@ -8358,14 +8270,14 @@
       </c>
     </row>
     <row r="75" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A75" s="4" t="s">
+      <c r="A75" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="B75" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C75" s="4"/>
-      <c r="D75" s="4" t="s">
+      <c r="C75" s="3"/>
+      <c r="D75" s="3" t="s">
         <v>113</v>
       </c>
       <c r="E75">
@@ -8451,14 +8363,14 @@
       </c>
     </row>
     <row r="76" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A76" s="4" t="s">
+      <c r="A76" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B76" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C76" s="4"/>
-      <c r="D76" s="4" t="s">
+      <c r="C76" s="3"/>
+      <c r="D76" s="3" t="s">
         <v>114</v>
       </c>
       <c r="E76">
@@ -8544,14 +8456,14 @@
       </c>
     </row>
     <row r="77" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A77" s="4" t="s">
+      <c r="A77" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="B77" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C77" s="4"/>
-      <c r="D77" s="4" t="s">
+      <c r="C77" s="3"/>
+      <c r="D77" s="3" t="s">
         <v>115</v>
       </c>
       <c r="E77">
@@ -8637,14 +8549,14 @@
       </c>
     </row>
     <row r="78" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A78" s="4" t="s">
+      <c r="A78" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B78" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C78" s="4"/>
-      <c r="D78" s="4" t="s">
+      <c r="C78" s="3"/>
+      <c r="D78" s="3" t="s">
         <v>116</v>
       </c>
       <c r="E78">
@@ -8730,14 +8642,14 @@
       </c>
     </row>
     <row r="79" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A79" s="4" t="s">
+      <c r="A79" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="B79" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C79" s="4"/>
-      <c r="D79" s="4" t="s">
+      <c r="C79" s="3"/>
+      <c r="D79" s="3" t="s">
         <v>117</v>
       </c>
       <c r="E79">
@@ -8823,14 +8735,14 @@
       </c>
     </row>
     <row r="80" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A80" s="4" t="s">
+      <c r="A80" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B80" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C80" s="4"/>
-      <c r="D80" s="4" t="s">
+      <c r="C80" s="3"/>
+      <c r="D80" s="3" t="s">
         <v>119</v>
       </c>
       <c r="E80">
@@ -8916,14 +8828,14 @@
       </c>
     </row>
     <row r="81" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A81" s="4" t="s">
+      <c r="A81" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="B81" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C81" s="4"/>
-      <c r="D81" s="4" t="s">
+      <c r="C81" s="3"/>
+      <c r="D81" s="3" t="s">
         <v>120</v>
       </c>
       <c r="E81">
@@ -9009,14 +8921,14 @@
       </c>
     </row>
     <row r="82" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A82" s="4" t="s">
+      <c r="A82" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B82" s="4" t="s">
+      <c r="B82" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C82" s="4"/>
-      <c r="D82" s="4" t="s">
+      <c r="C82" s="3"/>
+      <c r="D82" s="3" t="s">
         <v>121</v>
       </c>
       <c r="E82">
@@ -9102,14 +9014,14 @@
       </c>
     </row>
     <row r="83" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A83" s="4" t="s">
+      <c r="A83" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="B83" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C83" s="4"/>
-      <c r="D83" s="4" t="s">
+      <c r="C83" s="3"/>
+      <c r="D83" s="3" t="s">
         <v>123</v>
       </c>
       <c r="E83">
@@ -9195,16 +9107,16 @@
       </c>
     </row>
     <row r="84" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A84" s="4" t="s">
+      <c r="A84" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B84" s="4" t="s">
+      <c r="B84" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C84" s="4" t="s">
+      <c r="C84" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="D84" s="4" t="s">
+      <c r="D84" s="3" t="s">
         <v>125</v>
       </c>
       <c r="E84">
@@ -9290,16 +9202,16 @@
       </c>
     </row>
     <row r="85" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A85" s="4" t="s">
+      <c r="A85" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B85" s="4" t="s">
+      <c r="B85" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C85" s="4" t="s">
+      <c r="C85" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="D85" s="4" t="s">
+      <c r="D85" s="3" t="s">
         <v>126</v>
       </c>
       <c r="E85">
@@ -9385,16 +9297,16 @@
       </c>
     </row>
     <row r="86" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A86" s="4" t="s">
+      <c r="A86" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="B86" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C86" s="4" t="s">
+      <c r="C86" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="D86" s="4" t="s">
+      <c r="D86" s="3" t="s">
         <v>128</v>
       </c>
       <c r="E86">
@@ -9480,14 +9392,14 @@
       </c>
     </row>
     <row r="87" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A87" s="4" t="s">
+      <c r="A87" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B87" s="4" t="s">
+      <c r="B87" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C87" s="4"/>
-      <c r="D87" s="4" t="s">
+      <c r="C87" s="3"/>
+      <c r="D87" s="3" t="s">
         <v>129</v>
       </c>
       <c r="E87">
@@ -9573,16 +9485,16 @@
       </c>
     </row>
     <row r="88" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A88" s="4" t="s">
+      <c r="A88" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B88" s="4" t="s">
+      <c r="B88" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C88" s="4" t="s">
+      <c r="C88" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="D88" s="4" t="s">
+      <c r="D88" s="3" t="s">
         <v>130</v>
       </c>
       <c r="E88">
@@ -9668,14 +9580,14 @@
       </c>
     </row>
     <row r="89" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A89" s="4" t="s">
+      <c r="A89" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B89" s="4" t="s">
+      <c r="B89" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C89" s="4"/>
-      <c r="D89" s="4" t="s">
+      <c r="C89" s="3"/>
+      <c r="D89" s="3" t="s">
         <v>132</v>
       </c>
       <c r="E89">
@@ -9761,14 +9673,14 @@
       </c>
     </row>
     <row r="90" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A90" s="4" t="s">
+      <c r="A90" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B90" s="4" t="s">
+      <c r="B90" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C90" s="4"/>
-      <c r="D90" s="4" t="s">
+      <c r="C90" s="3"/>
+      <c r="D90" s="3" t="s">
         <v>133</v>
       </c>
       <c r="E90">
@@ -9854,14 +9766,14 @@
       </c>
     </row>
     <row r="91" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A91" s="4" t="s">
+      <c r="A91" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B91" s="4" t="s">
+      <c r="B91" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C91" s="4"/>
-      <c r="D91" s="4" t="s">
+      <c r="C91" s="3"/>
+      <c r="D91" s="3" t="s">
         <v>134</v>
       </c>
       <c r="E91">
@@ -9947,14 +9859,14 @@
       </c>
     </row>
     <row r="92" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A92" s="4" t="s">
+      <c r="A92" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B92" s="4" t="s">
+      <c r="B92" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C92" s="4"/>
-      <c r="D92" s="4" t="s">
+      <c r="C92" s="3"/>
+      <c r="D92" s="3" t="s">
         <v>135</v>
       </c>
       <c r="E92">
@@ -10040,14 +9952,14 @@
       </c>
     </row>
     <row r="93" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A93" s="4" t="s">
+      <c r="A93" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B93" s="4" t="s">
+      <c r="B93" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C93" s="4"/>
-      <c r="D93" s="4" t="s">
+      <c r="C93" s="3"/>
+      <c r="D93" s="3" t="s">
         <v>136</v>
       </c>
       <c r="E93">
@@ -10133,14 +10045,14 @@
       </c>
     </row>
     <row r="94" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A94" s="4" t="s">
+      <c r="A94" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B94" s="4" t="s">
+      <c r="B94" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="C94" s="4"/>
-      <c r="D94" s="4" t="s">
+      <c r="C94" s="3"/>
+      <c r="D94" s="3" t="s">
         <v>227</v>
       </c>
       <c r="E94">
@@ -10226,14 +10138,14 @@
       </c>
     </row>
     <row r="95" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A95" s="4" t="s">
+      <c r="A95" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="B95" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="C95" s="4"/>
-      <c r="D95" s="4" t="s">
+      <c r="C95" s="3"/>
+      <c r="D95" s="3" t="s">
         <v>228</v>
       </c>
       <c r="E95">
@@ -10319,15 +10231,15 @@
       </c>
     </row>
     <row r="96" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A96" s="4" t="s">
+      <c r="A96" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B96" s="4" t="s">
+      <c r="B96" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="C96" s="4"/>
-      <c r="D96" s="4" t="s">
-        <v>240</v>
+      <c r="C96" s="3"/>
+      <c r="D96" s="3" t="s">
+        <v>239</v>
       </c>
       <c r="E96">
         <v>2</v>
@@ -10412,15 +10324,15 @@
       </c>
     </row>
     <row r="97" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A97" s="4" t="s">
+      <c r="A97" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B97" s="4" t="s">
+      <c r="B97" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="C97" s="4"/>
-      <c r="D97" s="4" t="s">
-        <v>241</v>
+      <c r="C97" s="3"/>
+      <c r="D97" s="3" t="s">
+        <v>240</v>
       </c>
       <c r="E97">
         <v>2</v>
@@ -10505,14 +10417,14 @@
       </c>
     </row>
     <row r="98" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A98" s="4" t="s">
+      <c r="A98" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B98" s="4" t="s">
+      <c r="B98" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C98" s="4"/>
-      <c r="D98" s="4" t="s">
+      <c r="C98" s="3"/>
+      <c r="D98" s="3" t="s">
         <v>139</v>
       </c>
       <c r="E98">
@@ -10598,14 +10510,14 @@
       </c>
     </row>
     <row r="99" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A99" s="4" t="s">
+      <c r="A99" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B99" s="4" t="s">
+      <c r="B99" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C99" s="4"/>
-      <c r="D99" s="4" t="s">
+      <c r="C99" s="3"/>
+      <c r="D99" s="3" t="s">
         <v>140</v>
       </c>
       <c r="E99">
@@ -10691,14 +10603,14 @@
       </c>
     </row>
     <row r="100" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A100" s="4" t="s">
+      <c r="A100" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B100" s="4" t="s">
+      <c r="B100" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C100" s="4"/>
-      <c r="D100" s="4" t="s">
+      <c r="C100" s="3"/>
+      <c r="D100" s="3" t="s">
         <v>142</v>
       </c>
       <c r="E100">
@@ -10784,14 +10696,14 @@
       </c>
     </row>
     <row r="101" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A101" s="4" t="s">
+      <c r="A101" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B101" s="4" t="s">
+      <c r="B101" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C101" s="4"/>
-      <c r="D101" s="4" t="s">
+      <c r="C101" s="3"/>
+      <c r="D101" s="3" t="s">
         <v>143</v>
       </c>
       <c r="E101">
@@ -10877,14 +10789,14 @@
       </c>
     </row>
     <row r="102" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A102" s="4" t="s">
+      <c r="A102" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B102" s="4" t="s">
+      <c r="B102" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C102" s="4"/>
-      <c r="D102" s="4" t="s">
+      <c r="C102" s="3"/>
+      <c r="D102" s="3" t="s">
         <v>144</v>
       </c>
       <c r="E102">
@@ -10970,14 +10882,14 @@
       </c>
     </row>
     <row r="103" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A103" s="4" t="s">
+      <c r="A103" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B103" s="4" t="s">
+      <c r="B103" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C103" s="4"/>
-      <c r="D103" s="4" t="s">
+      <c r="C103" s="3"/>
+      <c r="D103" s="3" t="s">
         <v>145</v>
       </c>
       <c r="E103">
@@ -11063,14 +10975,14 @@
       </c>
     </row>
     <row r="104" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A104" s="4" t="s">
+      <c r="A104" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B104" s="4" t="s">
+      <c r="B104" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C104" s="4"/>
-      <c r="D104" s="4" t="s">
+      <c r="C104" s="3"/>
+      <c r="D104" s="3" t="s">
         <v>146</v>
       </c>
       <c r="E104">
@@ -11156,14 +11068,14 @@
       </c>
     </row>
     <row r="105" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A105" s="4" t="s">
+      <c r="A105" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B105" s="4" t="s">
+      <c r="B105" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C105" s="4"/>
-      <c r="D105" s="4" t="s">
+      <c r="C105" s="3"/>
+      <c r="D105" s="3" t="s">
         <v>147</v>
       </c>
       <c r="E105">
@@ -11249,14 +11161,14 @@
       </c>
     </row>
     <row r="106" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A106" s="4" t="s">
+      <c r="A106" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B106" s="4" t="s">
+      <c r="B106" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C106" s="4"/>
-      <c r="D106" s="4" t="s">
+      <c r="C106" s="3"/>
+      <c r="D106" s="3" t="s">
         <v>148</v>
       </c>
       <c r="E106">
@@ -11342,14 +11254,14 @@
       </c>
     </row>
     <row r="107" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A107" s="4" t="s">
+      <c r="A107" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B107" s="4" t="s">
+      <c r="B107" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C107" s="4"/>
-      <c r="D107" s="4" t="s">
+      <c r="C107" s="3"/>
+      <c r="D107" s="3" t="s">
         <v>149</v>
       </c>
       <c r="E107">
@@ -11435,14 +11347,14 @@
       </c>
     </row>
     <row r="108" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A108" s="4" t="s">
+      <c r="A108" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B108" s="4" t="s">
+      <c r="B108" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C108" s="4"/>
-      <c r="D108" s="4" t="s">
+      <c r="C108" s="3"/>
+      <c r="D108" s="3" t="s">
         <v>150</v>
       </c>
       <c r="E108">
@@ -11528,14 +11440,14 @@
       </c>
     </row>
     <row r="109" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A109" s="4" t="s">
+      <c r="A109" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B109" s="4" t="s">
+      <c r="B109" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C109" s="4"/>
-      <c r="D109" s="4" t="s">
+      <c r="C109" s="3"/>
+      <c r="D109" s="3" t="s">
         <v>151</v>
       </c>
       <c r="E109">
@@ -11621,14 +11533,14 @@
       </c>
     </row>
     <row r="110" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A110" s="4" t="s">
+      <c r="A110" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B110" s="4" t="s">
+      <c r="B110" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C110" s="4"/>
-      <c r="D110" s="4" t="s">
+      <c r="C110" s="3"/>
+      <c r="D110" s="3" t="s">
         <v>152</v>
       </c>
       <c r="E110">
@@ -11714,14 +11626,14 @@
       </c>
     </row>
     <row r="111" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A111" s="4" t="s">
+      <c r="A111" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B111" s="4" t="s">
+      <c r="B111" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C111" s="4"/>
-      <c r="D111" s="4" t="s">
+      <c r="C111" s="3"/>
+      <c r="D111" s="3" t="s">
         <v>153</v>
       </c>
       <c r="E111">
@@ -11807,14 +11719,14 @@
       </c>
     </row>
     <row r="112" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A112" s="4" t="s">
+      <c r="A112" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B112" s="4" t="s">
+      <c r="B112" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C112" s="4"/>
-      <c r="D112" s="4" t="s">
+      <c r="C112" s="3"/>
+      <c r="D112" s="3" t="s">
         <v>154</v>
       </c>
       <c r="E112">
@@ -11900,14 +11812,14 @@
       </c>
     </row>
     <row r="113" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A113" s="4" t="s">
+      <c r="A113" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B113" s="4" t="s">
+      <c r="B113" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C113" s="4"/>
-      <c r="D113" s="4" t="s">
+      <c r="C113" s="3"/>
+      <c r="D113" s="3" t="s">
         <v>155</v>
       </c>
       <c r="E113">
@@ -11993,14 +11905,14 @@
       </c>
     </row>
     <row r="114" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A114" s="4" t="s">
+      <c r="A114" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B114" s="4" t="s">
+      <c r="B114" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C114" s="4"/>
-      <c r="D114" s="4" t="s">
+      <c r="C114" s="3"/>
+      <c r="D114" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E114">
@@ -12086,14 +11998,14 @@
       </c>
     </row>
     <row r="115" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A115" s="4" t="s">
+      <c r="A115" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B115" s="4" t="s">
+      <c r="B115" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C115" s="4"/>
-      <c r="D115" s="4" t="s">
+      <c r="C115" s="3"/>
+      <c r="D115" s="3" t="s">
         <v>142</v>
       </c>
       <c r="E115">
@@ -12179,14 +12091,14 @@
       </c>
     </row>
     <row r="116" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A116" s="4" t="s">
+      <c r="A116" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B116" s="4" t="s">
+      <c r="B116" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C116" s="4"/>
-      <c r="D116" s="4" t="s">
+      <c r="C116" s="3"/>
+      <c r="D116" s="3" t="s">
         <v>143</v>
       </c>
       <c r="E116">
@@ -12272,14 +12184,14 @@
       </c>
     </row>
     <row r="117" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A117" s="4" t="s">
+      <c r="A117" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B117" s="4" t="s">
+      <c r="B117" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C117" s="4"/>
-      <c r="D117" s="4" t="s">
+      <c r="C117" s="3"/>
+      <c r="D117" s="3" t="s">
         <v>144</v>
       </c>
       <c r="E117">
@@ -12365,14 +12277,14 @@
       </c>
     </row>
     <row r="118" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A118" s="4" t="s">
+      <c r="A118" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B118" s="4" t="s">
+      <c r="B118" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C118" s="4"/>
-      <c r="D118" s="4" t="s">
+      <c r="C118" s="3"/>
+      <c r="D118" s="3" t="s">
         <v>145</v>
       </c>
       <c r="E118">
@@ -12458,14 +12370,14 @@
       </c>
     </row>
     <row r="119" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A119" s="4" t="s">
+      <c r="A119" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B119" s="4" t="s">
+      <c r="B119" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C119" s="4"/>
-      <c r="D119" s="4" t="s">
+      <c r="C119" s="3"/>
+      <c r="D119" s="3" t="s">
         <v>146</v>
       </c>
       <c r="E119">
@@ -12551,14 +12463,14 @@
       </c>
     </row>
     <row r="120" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A120" s="4" t="s">
+      <c r="A120" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B120" s="4" t="s">
+      <c r="B120" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C120" s="4"/>
-      <c r="D120" s="4" t="s">
+      <c r="C120" s="3"/>
+      <c r="D120" s="3" t="s">
         <v>147</v>
       </c>
       <c r="E120">
@@ -12644,14 +12556,14 @@
       </c>
     </row>
     <row r="121" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A121" s="4" t="s">
+      <c r="A121" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B121" s="4" t="s">
+      <c r="B121" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C121" s="4"/>
-      <c r="D121" s="4" t="s">
+      <c r="C121" s="3"/>
+      <c r="D121" s="3" t="s">
         <v>148</v>
       </c>
       <c r="E121">
@@ -12737,14 +12649,14 @@
       </c>
     </row>
     <row r="122" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A122" s="4" t="s">
+      <c r="A122" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B122" s="4" t="s">
+      <c r="B122" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C122" s="4"/>
-      <c r="D122" s="4" t="s">
+      <c r="C122" s="3"/>
+      <c r="D122" s="3" t="s">
         <v>149</v>
       </c>
       <c r="E122">
@@ -12830,14 +12742,14 @@
       </c>
     </row>
     <row r="123" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A123" s="4" t="s">
+      <c r="A123" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B123" s="4" t="s">
+      <c r="B123" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C123" s="4"/>
-      <c r="D123" s="4" t="s">
+      <c r="C123" s="3"/>
+      <c r="D123" s="3" t="s">
         <v>150</v>
       </c>
       <c r="E123">
@@ -12923,14 +12835,14 @@
       </c>
     </row>
     <row r="124" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A124" s="4" t="s">
+      <c r="A124" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B124" s="4" t="s">
+      <c r="B124" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C124" s="4"/>
-      <c r="D124" s="4" t="s">
+      <c r="C124" s="3"/>
+      <c r="D124" s="3" t="s">
         <v>151</v>
       </c>
       <c r="E124">
@@ -13016,14 +12928,14 @@
       </c>
     </row>
     <row r="125" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A125" s="4" t="s">
+      <c r="A125" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B125" s="4" t="s">
+      <c r="B125" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C125" s="4"/>
-      <c r="D125" s="4" t="s">
+      <c r="C125" s="3"/>
+      <c r="D125" s="3" t="s">
         <v>152</v>
       </c>
       <c r="E125">
@@ -13109,14 +13021,14 @@
       </c>
     </row>
     <row r="126" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A126" s="4" t="s">
+      <c r="A126" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B126" s="4" t="s">
+      <c r="B126" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C126" s="4"/>
-      <c r="D126" s="4" t="s">
+      <c r="C126" s="3"/>
+      <c r="D126" s="3" t="s">
         <v>153</v>
       </c>
       <c r="E126">
@@ -13202,14 +13114,14 @@
       </c>
     </row>
     <row r="127" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A127" s="4" t="s">
+      <c r="A127" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B127" s="4" t="s">
+      <c r="B127" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C127" s="4"/>
-      <c r="D127" s="4" t="s">
+      <c r="C127" s="3"/>
+      <c r="D127" s="3" t="s">
         <v>154</v>
       </c>
       <c r="E127">
@@ -13295,14 +13207,14 @@
       </c>
     </row>
     <row r="128" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A128" s="4" t="s">
+      <c r="A128" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B128" s="4" t="s">
+      <c r="B128" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C128" s="4"/>
-      <c r="D128" s="4" t="s">
+      <c r="C128" s="3"/>
+      <c r="D128" s="3" t="s">
         <v>155</v>
       </c>
       <c r="E128">
@@ -13388,14 +13300,14 @@
       </c>
     </row>
     <row r="129" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A129" s="4" t="s">
+      <c r="A129" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B129" s="4" t="s">
+      <c r="B129" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C129" s="4"/>
-      <c r="D129" s="4" t="s">
+      <c r="C129" s="3"/>
+      <c r="D129" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E129">
@@ -13481,14 +13393,14 @@
       </c>
     </row>
     <row r="130" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A130" s="4" t="s">
+      <c r="A130" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B130" s="4" t="s">
+      <c r="B130" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C130" s="4"/>
-      <c r="D130" s="4" t="s">
+      <c r="C130" s="3"/>
+      <c r="D130" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E130">
@@ -13574,14 +13486,14 @@
       </c>
     </row>
     <row r="131" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A131" s="4" t="s">
+      <c r="A131" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B131" s="4" t="s">
+      <c r="B131" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C131" s="4"/>
-      <c r="D131" s="4" t="s">
+      <c r="C131" s="3"/>
+      <c r="D131" s="3" t="s">
         <v>160</v>
       </c>
       <c r="E131">
@@ -13667,16 +13579,16 @@
       </c>
     </row>
     <row r="132" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A132" s="4" t="s">
+      <c r="A132" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B132" s="4" t="s">
+      <c r="B132" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="C132" s="4" t="s">
+      <c r="C132" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="D132" s="4" t="s">
+      <c r="D132" s="3" t="s">
         <v>163</v>
       </c>
       <c r="E132">
@@ -13762,16 +13674,16 @@
       </c>
     </row>
     <row r="133" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A133" s="4" t="s">
+      <c r="A133" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B133" s="4" t="s">
+      <c r="B133" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="C133" s="4" t="s">
+      <c r="C133" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="D133" s="4" t="s">
+      <c r="D133" s="3" t="s">
         <v>164</v>
       </c>
       <c r="E133">
@@ -13857,16 +13769,16 @@
       </c>
     </row>
     <row r="134" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A134" s="4" t="s">
+      <c r="A134" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B134" s="4" t="s">
+      <c r="B134" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="C134" s="4" t="s">
+      <c r="C134" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="D134" s="4" t="s">
+      <c r="D134" s="3" t="s">
         <v>165</v>
       </c>
       <c r="E134">
@@ -13952,16 +13864,16 @@
       </c>
     </row>
     <row r="135" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A135" s="4" t="s">
+      <c r="A135" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B135" s="4" t="s">
+      <c r="B135" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="C135" s="4" t="s">
+      <c r="C135" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="D135" s="4" t="s">
+      <c r="D135" s="3" t="s">
         <v>166</v>
       </c>
       <c r="E135">
@@ -14047,16 +13959,16 @@
       </c>
     </row>
     <row r="136" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A136" s="4" t="s">
+      <c r="A136" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B136" s="4" t="s">
+      <c r="B136" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="C136" s="4" t="s">
+      <c r="C136" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="D136" s="4" t="s">
+      <c r="D136" s="3" t="s">
         <v>145</v>
       </c>
       <c r="E136">
@@ -14142,16 +14054,16 @@
       </c>
     </row>
     <row r="137" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A137" s="4" t="s">
+      <c r="A137" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B137" s="4" t="s">
+      <c r="B137" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="C137" s="4" t="s">
+      <c r="C137" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="D137" s="4" t="s">
+      <c r="D137" s="3" t="s">
         <v>168</v>
       </c>
       <c r="E137">
@@ -14237,16 +14149,16 @@
       </c>
     </row>
     <row r="138" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A138" s="4" t="s">
+      <c r="A138" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B138" s="4" t="s">
+      <c r="B138" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="C138" s="4" t="s">
+      <c r="C138" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="D138" s="4" t="s">
+      <c r="D138" s="3" t="s">
         <v>169</v>
       </c>
       <c r="E138">
@@ -14332,16 +14244,16 @@
       </c>
     </row>
     <row r="139" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A139" s="4" t="s">
+      <c r="A139" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B139" s="4" t="s">
+      <c r="B139" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="C139" s="4" t="s">
+      <c r="C139" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="D139" s="4" t="s">
+      <c r="D139" s="3" t="s">
         <v>170</v>
       </c>
       <c r="E139">
@@ -14427,16 +14339,16 @@
       </c>
     </row>
     <row r="140" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A140" s="4" t="s">
+      <c r="A140" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B140" s="4" t="s">
+      <c r="B140" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="C140" s="4" t="s">
+      <c r="C140" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="D140" s="4" t="s">
+      <c r="D140" s="3" t="s">
         <v>171</v>
       </c>
       <c r="E140">
@@ -14522,16 +14434,16 @@
       </c>
     </row>
     <row r="141" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A141" s="4" t="s">
+      <c r="A141" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B141" s="4" t="s">
+      <c r="B141" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="C141" s="4" t="s">
+      <c r="C141" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="D141" s="4" t="s">
+      <c r="D141" s="3" t="s">
         <v>142</v>
       </c>
       <c r="E141">
@@ -14617,16 +14529,16 @@
       </c>
     </row>
     <row r="142" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A142" s="4" t="s">
+      <c r="A142" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B142" s="4" t="s">
+      <c r="B142" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="C142" s="4" t="s">
+      <c r="C142" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="D142" s="4" t="s">
+      <c r="D142" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E142">
@@ -14712,16 +14624,16 @@
       </c>
     </row>
     <row r="143" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A143" s="4" t="s">
+      <c r="A143" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B143" s="4" t="s">
+      <c r="B143" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="C143" s="4" t="s">
+      <c r="C143" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="D143" s="4" t="s">
+      <c r="D143" s="3" t="s">
         <v>172</v>
       </c>
       <c r="E143">
@@ -14807,16 +14719,16 @@
       </c>
     </row>
     <row r="144" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A144" s="4" t="s">
+      <c r="A144" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B144" s="4" t="s">
+      <c r="B144" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="C144" s="4" t="s">
+      <c r="C144" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="D144" s="4" t="s">
+      <c r="D144" s="3" t="s">
         <v>175</v>
       </c>
       <c r="E144">
@@ -14902,16 +14814,16 @@
       </c>
     </row>
     <row r="145" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A145" s="4" t="s">
+      <c r="A145" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B145" s="4" t="s">
+      <c r="B145" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="C145" s="4" t="s">
+      <c r="C145" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="D145" s="4" t="s">
+      <c r="D145" s="3" t="s">
         <v>176</v>
       </c>
       <c r="E145">
@@ -14997,16 +14909,16 @@
       </c>
     </row>
     <row r="146" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A146" s="4" t="s">
+      <c r="A146" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B146" s="4" t="s">
+      <c r="B146" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="C146" s="4" t="s">
+      <c r="C146" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="D146" s="4" t="s">
+      <c r="D146" s="3" t="s">
         <v>177</v>
       </c>
       <c r="E146">
@@ -15092,16 +15004,16 @@
       </c>
     </row>
     <row r="147" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A147" s="4" t="s">
+      <c r="A147" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B147" s="4" t="s">
+      <c r="B147" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="C147" s="4" t="s">
+      <c r="C147" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="D147" s="4" t="s">
+      <c r="D147" s="3" t="s">
         <v>178</v>
       </c>
       <c r="E147">
@@ -15187,16 +15099,16 @@
       </c>
     </row>
     <row r="148" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A148" s="4" t="s">
+      <c r="A148" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B148" s="4" t="s">
+      <c r="B148" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="C148" s="4" t="s">
+      <c r="C148" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="D148" s="4" t="s">
+      <c r="D148" s="3" t="s">
         <v>179</v>
       </c>
       <c r="E148">
@@ -15282,16 +15194,16 @@
       </c>
     </row>
     <row r="149" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A149" s="4" t="s">
+      <c r="A149" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B149" s="4" t="s">
+      <c r="B149" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="C149" s="4" t="s">
+      <c r="C149" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="D149" s="4" t="s">
+      <c r="D149" s="3" t="s">
         <v>181</v>
       </c>
       <c r="E149">
@@ -15377,16 +15289,16 @@
       </c>
     </row>
     <row r="150" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A150" s="4" t="s">
+      <c r="A150" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B150" s="4" t="s">
+      <c r="B150" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="C150" s="4" t="s">
+      <c r="C150" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="D150" s="4" t="s">
+      <c r="D150" s="3" t="s">
         <v>178</v>
       </c>
       <c r="E150">
@@ -15472,16 +15384,16 @@
       </c>
     </row>
     <row r="151" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A151" s="4" t="s">
+      <c r="A151" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B151" s="4" t="s">
+      <c r="B151" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="C151" s="4" t="s">
+      <c r="C151" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="D151" s="4" t="s">
+      <c r="D151" s="3" t="s">
         <v>179</v>
       </c>
       <c r="E151">
@@ -15567,14 +15479,14 @@
       </c>
     </row>
     <row r="152" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A152" s="4" t="s">
+      <c r="A152" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B152" s="4" t="s">
+      <c r="B152" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="C152" s="4"/>
-      <c r="D152" s="4" t="s">
+      <c r="C152" s="3"/>
+      <c r="D152" s="3" t="s">
         <v>142</v>
       </c>
       <c r="E152">
@@ -15660,14 +15572,14 @@
       </c>
     </row>
     <row r="153" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A153" s="4" t="s">
+      <c r="A153" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B153" s="4" t="s">
+      <c r="B153" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="C153" s="4"/>
-      <c r="D153" s="4" t="s">
+      <c r="C153" s="3"/>
+      <c r="D153" s="3" t="s">
         <v>143</v>
       </c>
       <c r="E153">
@@ -15753,14 +15665,14 @@
       </c>
     </row>
     <row r="154" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A154" s="4" t="s">
+      <c r="A154" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B154" s="4" t="s">
+      <c r="B154" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="C154" s="4"/>
-      <c r="D154" s="4" t="s">
+      <c r="C154" s="3"/>
+      <c r="D154" s="3" t="s">
         <v>144</v>
       </c>
       <c r="E154">
@@ -15846,14 +15758,14 @@
       </c>
     </row>
     <row r="155" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A155" s="4" t="s">
+      <c r="A155" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B155" s="4" t="s">
+      <c r="B155" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="C155" s="4"/>
-      <c r="D155" s="4" t="s">
+      <c r="C155" s="3"/>
+      <c r="D155" s="3" t="s">
         <v>145</v>
       </c>
       <c r="E155">
@@ -15939,14 +15851,14 @@
       </c>
     </row>
     <row r="156" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A156" s="4" t="s">
+      <c r="A156" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B156" s="4" t="s">
+      <c r="B156" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="C156" s="4"/>
-      <c r="D156" s="4" t="s">
+      <c r="C156" s="3"/>
+      <c r="D156" s="3" t="s">
         <v>146</v>
       </c>
       <c r="E156">
@@ -16032,14 +15944,14 @@
       </c>
     </row>
     <row r="157" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A157" s="4" t="s">
+      <c r="A157" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B157" s="4" t="s">
+      <c r="B157" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="C157" s="4"/>
-      <c r="D157" s="4" t="s">
+      <c r="C157" s="3"/>
+      <c r="D157" s="3" t="s">
         <v>147</v>
       </c>
       <c r="E157">
@@ -16125,14 +16037,14 @@
       </c>
     </row>
     <row r="158" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A158" s="4" t="s">
+      <c r="A158" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B158" s="4" t="s">
+      <c r="B158" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="C158" s="4"/>
-      <c r="D158" s="4" t="s">
+      <c r="C158" s="3"/>
+      <c r="D158" s="3" t="s">
         <v>148</v>
       </c>
       <c r="E158">
@@ -16218,14 +16130,14 @@
       </c>
     </row>
     <row r="159" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A159" s="4" t="s">
+      <c r="A159" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B159" s="4" t="s">
+      <c r="B159" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="C159" s="4"/>
-      <c r="D159" s="4" t="s">
+      <c r="C159" s="3"/>
+      <c r="D159" s="3" t="s">
         <v>149</v>
       </c>
       <c r="E159">
@@ -16311,14 +16223,14 @@
       </c>
     </row>
     <row r="160" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A160" s="4" t="s">
+      <c r="A160" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B160" s="4" t="s">
+      <c r="B160" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="C160" s="4"/>
-      <c r="D160" s="4" t="s">
+      <c r="C160" s="3"/>
+      <c r="D160" s="3" t="s">
         <v>150</v>
       </c>
       <c r="E160">
@@ -16404,14 +16316,14 @@
       </c>
     </row>
     <row r="161" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A161" s="4" t="s">
+      <c r="A161" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B161" s="4" t="s">
+      <c r="B161" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="C161" s="4"/>
-      <c r="D161" s="4" t="s">
+      <c r="C161" s="3"/>
+      <c r="D161" s="3" t="s">
         <v>151</v>
       </c>
       <c r="E161">
@@ -16497,14 +16409,14 @@
       </c>
     </row>
     <row r="162" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A162" s="4" t="s">
+      <c r="A162" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B162" s="4" t="s">
+      <c r="B162" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="C162" s="4"/>
-      <c r="D162" s="4" t="s">
+      <c r="C162" s="3"/>
+      <c r="D162" s="3" t="s">
         <v>152</v>
       </c>
       <c r="E162">
@@ -16590,14 +16502,14 @@
       </c>
     </row>
     <row r="163" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A163" s="4" t="s">
+      <c r="A163" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B163" s="4" t="s">
+      <c r="B163" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="C163" s="4"/>
-      <c r="D163" s="4" t="s">
+      <c r="C163" s="3"/>
+      <c r="D163" s="3" t="s">
         <v>153</v>
       </c>
       <c r="E163">
@@ -16683,14 +16595,14 @@
       </c>
     </row>
     <row r="164" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A164" s="4" t="s">
+      <c r="A164" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B164" s="4" t="s">
+      <c r="B164" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="C164" s="4"/>
-      <c r="D164" s="4" t="s">
+      <c r="C164" s="3"/>
+      <c r="D164" s="3" t="s">
         <v>154</v>
       </c>
       <c r="E164">
@@ -16776,14 +16688,14 @@
       </c>
     </row>
     <row r="165" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A165" s="4" t="s">
+      <c r="A165" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B165" s="4" t="s">
+      <c r="B165" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="C165" s="4"/>
-      <c r="D165" s="4" t="s">
+      <c r="C165" s="3"/>
+      <c r="D165" s="3" t="s">
         <v>155</v>
       </c>
       <c r="E165">
@@ -16869,14 +16781,14 @@
       </c>
     </row>
     <row r="166" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A166" s="4" t="s">
+      <c r="A166" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B166" s="4" t="s">
+      <c r="B166" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="C166" s="4"/>
-      <c r="D166" s="4" t="s">
+      <c r="C166" s="3"/>
+      <c r="D166" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E166">
@@ -16962,16 +16874,16 @@
       </c>
     </row>
     <row r="167" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A167" s="4" t="s">
+      <c r="A167" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B167" s="4" t="s">
+      <c r="B167" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="C167" s="4" t="s">
+      <c r="C167" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="D167" s="4" t="s">
+      <c r="D167" s="3" t="s">
         <v>185</v>
       </c>
       <c r="E167">
@@ -17057,16 +16969,16 @@
       </c>
     </row>
     <row r="168" spans="1:31" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A168" s="4" t="s">
+      <c r="A168" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B168" s="4" t="s">
+      <c r="B168" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="C168" s="4" t="s">
+      <c r="C168" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="D168" s="4" t="s">
+      <c r="D168" s="3" t="s">
         <v>186</v>
       </c>
       <c r="E168">
@@ -17152,16 +17064,16 @@
       </c>
     </row>
     <row r="169" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A169" s="4" t="s">
+      <c r="A169" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B169" s="4" t="s">
+      <c r="B169" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="C169" s="4" t="s">
+      <c r="C169" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="D169" s="4" t="s">
+      <c r="D169" s="3" t="s">
         <v>185</v>
       </c>
       <c r="E169">
@@ -17247,16 +17159,16 @@
       </c>
     </row>
     <row r="170" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A170" s="4" t="s">
+      <c r="A170" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B170" s="4" t="s">
+      <c r="B170" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="C170" s="4" t="s">
+      <c r="C170" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="D170" s="4" t="s">
+      <c r="D170" s="3" t="s">
         <v>186</v>
       </c>
       <c r="E170">
@@ -17342,15 +17254,15 @@
       </c>
     </row>
     <row r="171" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A171" s="4" t="s">
+      <c r="A171" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B171" s="4" t="s">
+      <c r="B171" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="C171" s="4"/>
-      <c r="D171" s="4" t="s">
-        <v>242</v>
+      <c r="C171" s="3"/>
+      <c r="D171" s="3" t="s">
+        <v>241</v>
       </c>
       <c r="E171">
         <v>4</v>
@@ -17435,14 +17347,14 @@
       </c>
     </row>
     <row r="172" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A172" s="4" t="s">
+      <c r="A172" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B172" s="4" t="s">
+      <c r="B172" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="C172" s="4"/>
-      <c r="D172" s="4" t="s">
+      <c r="C172" s="3"/>
+      <c r="D172" s="3" t="s">
         <v>190</v>
       </c>
       <c r="E172">
@@ -17528,16 +17440,16 @@
       </c>
     </row>
     <row r="173" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A173" s="4" t="s">
+      <c r="A173" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B173" s="4" t="s">
+      <c r="B173" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="C173" s="4" t="s">
+      <c r="C173" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="D173" s="4" t="s">
+      <c r="D173" s="3" t="s">
         <v>193</v>
       </c>
       <c r="E173">
@@ -17623,16 +17535,16 @@
       </c>
     </row>
     <row r="174" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A174" s="4" t="s">
+      <c r="A174" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B174" s="4" t="s">
+      <c r="B174" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="C174" s="4" t="s">
+      <c r="C174" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="D174" s="4" t="s">
+      <c r="D174" s="3" t="s">
         <v>194</v>
       </c>
       <c r="E174">
@@ -17718,16 +17630,16 @@
       </c>
     </row>
     <row r="175" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A175" s="4" t="s">
+      <c r="A175" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B175" s="4" t="s">
+      <c r="B175" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="C175" s="4" t="s">
+      <c r="C175" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="D175" s="4" t="s">
+      <c r="D175" s="3" t="s">
         <v>195</v>
       </c>
       <c r="E175">
@@ -17813,16 +17725,16 @@
       </c>
     </row>
     <row r="176" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A176" s="4" t="s">
+      <c r="A176" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B176" s="4" t="s">
+      <c r="B176" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="C176" s="4" t="s">
+      <c r="C176" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="D176" s="4" t="s">
+      <c r="D176" s="3" t="s">
         <v>196</v>
       </c>
       <c r="E176">
@@ -17908,16 +17820,16 @@
       </c>
     </row>
     <row r="177" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A177" s="4" t="s">
+      <c r="A177" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B177" s="4" t="s">
+      <c r="B177" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="C177" s="4" t="s">
+      <c r="C177" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="D177" s="4" t="s">
+      <c r="D177" s="3" t="s">
         <v>197</v>
       </c>
       <c r="E177">
@@ -18003,16 +17915,16 @@
       </c>
     </row>
     <row r="178" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A178" s="4" t="s">
+      <c r="A178" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B178" s="4" t="s">
+      <c r="B178" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="C178" s="4" t="s">
+      <c r="C178" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="D178" s="4" t="s">
+      <c r="D178" s="3" t="s">
         <v>199</v>
       </c>
       <c r="E178">
@@ -18098,16 +18010,16 @@
       </c>
     </row>
     <row r="179" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A179" s="4" t="s">
+      <c r="A179" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B179" s="4" t="s">
+      <c r="B179" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="C179" s="4" t="s">
+      <c r="C179" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="D179" s="4" t="s">
+      <c r="D179" s="3" t="s">
         <v>200</v>
       </c>
       <c r="E179">
@@ -18193,14 +18105,14 @@
       </c>
     </row>
     <row r="180" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A180" s="4" t="s">
+      <c r="A180" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B180" s="4" t="s">
+      <c r="B180" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="C180" s="4"/>
-      <c r="D180" s="4" t="s">
+      <c r="C180" s="3"/>
+      <c r="D180" s="3" t="s">
         <v>202</v>
       </c>
       <c r="E180">
@@ -18286,14 +18198,14 @@
       </c>
     </row>
     <row r="181" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A181" s="4" t="s">
+      <c r="A181" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B181" s="4" t="s">
+      <c r="B181" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="C181" s="4"/>
-      <c r="D181" s="4" t="s">
+      <c r="C181" s="3"/>
+      <c r="D181" s="3" t="s">
         <v>203</v>
       </c>
       <c r="E181">
@@ -18379,16 +18291,16 @@
       </c>
     </row>
     <row r="182" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A182" s="4" t="s">
+      <c r="A182" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B182" s="4" t="s">
+      <c r="B182" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="C182" s="4" t="s">
+      <c r="C182" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="D182" s="4" t="s">
+      <c r="D182" s="3" t="s">
         <v>206</v>
       </c>
       <c r="E182">
@@ -18474,16 +18386,16 @@
       </c>
     </row>
     <row r="183" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A183" s="4" t="s">
+      <c r="A183" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B183" s="4" t="s">
+      <c r="B183" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="C183" s="4" t="s">
+      <c r="C183" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="D183" s="4" t="s">
+      <c r="D183" s="3" t="s">
         <v>207</v>
       </c>
       <c r="E183">
@@ -18569,16 +18481,16 @@
       </c>
     </row>
     <row r="184" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A184" s="4" t="s">
+      <c r="A184" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B184" s="4" t="s">
+      <c r="B184" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="C184" s="4" t="s">
+      <c r="C184" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="D184" s="4" t="s">
+      <c r="D184" s="3" t="s">
         <v>208</v>
       </c>
       <c r="E184">
@@ -18664,16 +18576,16 @@
       </c>
     </row>
     <row r="185" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A185" s="4" t="s">
+      <c r="A185" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B185" s="4" t="s">
+      <c r="B185" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="C185" s="4" t="s">
+      <c r="C185" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="D185" s="4" t="s">
+      <c r="D185" s="3" t="s">
         <v>209</v>
       </c>
       <c r="E185">
@@ -18759,16 +18671,16 @@
       </c>
     </row>
     <row r="186" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A186" s="4" t="s">
+      <c r="A186" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B186" s="4" t="s">
+      <c r="B186" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="C186" s="4" t="s">
+      <c r="C186" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="D186" s="4" t="s">
+      <c r="D186" s="3" t="s">
         <v>210</v>
       </c>
       <c r="E186">
@@ -18854,16 +18766,16 @@
       </c>
     </row>
     <row r="187" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A187" s="4" t="s">
+      <c r="A187" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B187" s="4" t="s">
+      <c r="B187" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="C187" s="4" t="s">
+      <c r="C187" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="D187" s="4" t="s">
+      <c r="D187" s="3" t="s">
         <v>211</v>
       </c>
       <c r="E187">
@@ -18949,16 +18861,16 @@
       </c>
     </row>
     <row r="188" spans="1:31" ht="48" x14ac:dyDescent="0.2">
-      <c r="A188" s="4" t="s">
+      <c r="A188" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B188" s="4" t="s">
+      <c r="B188" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="C188" s="4" t="s">
+      <c r="C188" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="D188" s="5" t="s">
+      <c r="D188" s="4" t="s">
         <v>212</v>
       </c>
       <c r="E188">
@@ -19044,16 +18956,16 @@
       </c>
     </row>
     <row r="189" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A189" s="4" t="s">
+      <c r="A189" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B189" s="4" t="s">
+      <c r="B189" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="C189" s="4" t="s">
+      <c r="C189" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="D189" s="4" t="s">
+      <c r="D189" s="3" t="s">
         <v>214</v>
       </c>
       <c r="E189">
@@ -19139,16 +19051,16 @@
       </c>
     </row>
     <row r="190" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A190" s="4" t="s">
+      <c r="A190" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B190" s="4" t="s">
+      <c r="B190" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="C190" s="4" t="s">
+      <c r="C190" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="D190" s="4" t="s">
+      <c r="D190" s="3" t="s">
         <v>216</v>
       </c>
       <c r="E190">
@@ -19234,16 +19146,16 @@
       </c>
     </row>
     <row r="191" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A191" s="4" t="s">
+      <c r="A191" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B191" s="4" t="s">
+      <c r="B191" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="C191" s="4" t="s">
+      <c r="C191" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="D191" s="4" t="s">
+      <c r="D191" s="3" t="s">
         <v>217</v>
       </c>
       <c r="E191">
@@ -19329,16 +19241,16 @@
       </c>
     </row>
     <row r="192" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A192" s="4" t="s">
+      <c r="A192" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B192" s="4" t="s">
+      <c r="B192" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="C192" s="4" t="s">
+      <c r="C192" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="D192" s="4" t="s">
+      <c r="D192" s="3" t="s">
         <v>218</v>
       </c>
       <c r="E192">
@@ -19424,16 +19336,16 @@
       </c>
     </row>
     <row r="193" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A193" s="4" t="s">
+      <c r="A193" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B193" s="4" t="s">
+      <c r="B193" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="C193" s="4" t="s">
+      <c r="C193" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="D193" s="4" t="s">
+      <c r="D193" s="3" t="s">
         <v>219</v>
       </c>
       <c r="E193">
@@ -19519,14 +19431,14 @@
       </c>
     </row>
     <row r="194" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A194" s="4" t="s">
+      <c r="A194" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B194" s="4" t="s">
+      <c r="B194" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="C194" s="4"/>
-      <c r="D194" s="4" t="s">
+      <c r="C194" s="3"/>
+      <c r="D194" s="3" t="s">
         <v>229</v>
       </c>
       <c r="E194">
@@ -19612,14 +19524,14 @@
       </c>
     </row>
     <row r="195" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A195" s="4" t="s">
+      <c r="A195" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B195" s="4" t="s">
+      <c r="B195" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="C195" s="4"/>
-      <c r="D195" s="4" t="s">
+      <c r="C195" s="3"/>
+      <c r="D195" s="3" t="s">
         <v>230</v>
       </c>
       <c r="E195">
@@ -19705,14 +19617,14 @@
       </c>
     </row>
     <row r="196" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A196" s="4" t="s">
+      <c r="A196" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B196" s="4" t="s">
+      <c r="B196" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="C196" s="4"/>
-      <c r="D196" s="4" t="s">
+      <c r="C196" s="3"/>
+      <c r="D196" s="3" t="s">
         <v>231</v>
       </c>
       <c r="E196">
@@ -19798,14 +19710,14 @@
       </c>
     </row>
     <row r="197" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A197" s="4" t="s">
+      <c r="A197" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B197" s="4" t="s">
+      <c r="B197" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="C197" s="4"/>
-      <c r="D197" s="4" t="s">
+      <c r="C197" s="3"/>
+      <c r="D197" s="3" t="s">
         <v>177</v>
       </c>
       <c r="E197">
@@ -19891,14 +19803,14 @@
       </c>
     </row>
     <row r="198" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A198" s="4" t="s">
+      <c r="A198" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B198" s="4" t="s">
+      <c r="B198" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="C198" s="4"/>
-      <c r="D198" s="4" t="s">
+      <c r="C198" s="3"/>
+      <c r="D198" s="3" t="s">
         <v>232</v>
       </c>
       <c r="E198">
@@ -19984,15 +19896,15 @@
       </c>
     </row>
     <row r="199" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A199" s="4" t="s">
+      <c r="A199" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B199" s="4" t="s">
+      <c r="B199" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="C199" s="4"/>
-      <c r="D199" s="4" t="s">
-        <v>242</v>
+      <c r="C199" s="3"/>
+      <c r="D199" s="3" t="s">
+        <v>241</v>
       </c>
       <c r="E199">
         <v>2</v>
@@ -20077,13 +19989,13 @@
       </c>
     </row>
     <row r="200" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A200" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="B200" s="6"/>
-      <c r="C200" s="6"/>
-      <c r="D200" s="6" t="s">
-        <v>243</v>
+      <c r="A200" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="B200" s="5"/>
+      <c r="C200" s="5"/>
+      <c r="D200" s="5" t="s">
+        <v>242</v>
       </c>
       <c r="E200">
         <v>3</v>
@@ -20168,12 +20080,12 @@
       </c>
     </row>
     <row r="201" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A201" s="4" t="s">
+      <c r="A201" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="B201" s="4"/>
-      <c r="C201" s="4"/>
-      <c r="D201" s="4" t="s">
+      <c r="B201" s="3"/>
+      <c r="C201" s="3"/>
+      <c r="D201" s="3" t="s">
         <v>221</v>
       </c>
       <c r="E201">
@@ -20259,12 +20171,12 @@
       </c>
     </row>
     <row r="202" spans="1:31" ht="15" x14ac:dyDescent="0.2">
-      <c r="A202" s="4" t="s">
+      <c r="A202" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="B202" s="4"/>
-      <c r="C202" s="4"/>
-      <c r="D202" s="4" t="s">
+      <c r="B202" s="3"/>
+      <c r="C202" s="3"/>
+      <c r="D202" s="3" t="s">
         <v>222</v>
       </c>
       <c r="E202">
@@ -20350,12 +20262,12 @@
       </c>
     </row>
     <row r="203" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A203" s="4" t="s">
+      <c r="A203" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="B203" s="4"/>
-      <c r="C203" s="4"/>
-      <c r="D203" s="4" t="s">
+      <c r="B203" s="3"/>
+      <c r="C203" s="3"/>
+      <c r="D203" s="3" t="s">
         <v>223</v>
       </c>
       <c r="E203">
@@ -20441,12 +20353,12 @@
       </c>
     </row>
     <row r="204" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A204" s="4" t="s">
+      <c r="A204" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="B204" s="4"/>
-      <c r="C204" s="4"/>
-      <c r="D204" s="4" t="s">
+      <c r="B204" s="3"/>
+      <c r="C204" s="3"/>
+      <c r="D204" s="3" t="s">
         <v>224</v>
       </c>
       <c r="E204">
@@ -20532,12 +20444,12 @@
       </c>
     </row>
     <row r="205" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A205" s="4" t="s">
+      <c r="A205" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="B205" s="4"/>
-      <c r="C205" s="4"/>
-      <c r="D205" s="4" t="s">
+      <c r="B205" s="3"/>
+      <c r="C205" s="3"/>
+      <c r="D205" s="3" t="s">
         <v>225</v>
       </c>
       <c r="E205">
@@ -20623,10 +20535,10 @@
       </c>
     </row>
     <row r="206" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A206" s="4"/>
-      <c r="B206" s="4"/>
-      <c r="C206" s="4"/>
-      <c r="D206" s="4"/>
+      <c r="A206" s="3"/>
+      <c r="B206" s="3"/>
+      <c r="C206" s="3"/>
+      <c r="D206" s="3"/>
       <c r="E206">
         <v>2</v>
       </c>
@@ -20710,10 +20622,10 @@
       </c>
     </row>
     <row r="207" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A207" s="4"/>
-      <c r="B207" s="4"/>
-      <c r="C207" s="4"/>
-      <c r="D207" s="4"/>
+      <c r="A207" s="3"/>
+      <c r="B207" s="3"/>
+      <c r="C207" s="3"/>
+      <c r="D207" s="3"/>
       <c r="E207">
         <v>2</v>
       </c>
@@ -20797,10 +20709,10 @@
       </c>
     </row>
     <row r="208" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A208" s="4"/>
-      <c r="B208" s="4"/>
-      <c r="C208" s="4"/>
-      <c r="D208" s="4"/>
+      <c r="A208" s="3"/>
+      <c r="B208" s="3"/>
+      <c r="C208" s="3"/>
+      <c r="D208" s="3"/>
       <c r="E208">
         <v>2</v>
       </c>
@@ -20884,10 +20796,10 @@
       </c>
     </row>
     <row r="209" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A209" s="4"/>
-      <c r="B209" s="4"/>
-      <c r="C209" s="4"/>
-      <c r="D209" s="4"/>
+      <c r="A209" s="3"/>
+      <c r="B209" s="3"/>
+      <c r="C209" s="3"/>
+      <c r="D209" s="3"/>
       <c r="E209">
         <v>2</v>
       </c>
@@ -20971,10 +20883,10 @@
       </c>
     </row>
     <row r="210" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A210" s="4"/>
-      <c r="B210" s="6"/>
-      <c r="C210" s="6"/>
-      <c r="D210" s="6"/>
+      <c r="A210" s="3"/>
+      <c r="B210" s="5"/>
+      <c r="C210" s="5"/>
+      <c r="D210" s="5"/>
       <c r="E210">
         <v>3.2</v>
       </c>
@@ -21058,14 +20970,14 @@
       </c>
     </row>
     <row r="211" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A211" s="4" t="s">
+      <c r="A211" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="B211" s="4" t="s">
+      <c r="B211" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="C211" s="4"/>
-      <c r="D211" s="4" t="s">
+      <c r="C211" s="3"/>
+      <c r="D211" s="3" t="s">
         <v>229</v>
       </c>
       <c r="E211">
@@ -21151,14 +21063,14 @@
       </c>
     </row>
     <row r="212" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A212" s="4" t="s">
+      <c r="A212" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="B212" s="4" t="s">
+      <c r="B212" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="C212" s="4"/>
-      <c r="D212" s="4" t="s">
+      <c r="C212" s="3"/>
+      <c r="D212" s="3" t="s">
         <v>177</v>
       </c>
       <c r="E212">
@@ -21244,14 +21156,14 @@
       </c>
     </row>
     <row r="213" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A213" s="4" t="s">
+      <c r="A213" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="B213" s="4" t="s">
+      <c r="B213" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="C213" s="4"/>
-      <c r="D213" s="4" t="s">
+      <c r="C213" s="3"/>
+      <c r="D213" s="3" t="s">
         <v>235</v>
       </c>
       <c r="E213">
@@ -21337,14 +21249,14 @@
       </c>
     </row>
     <row r="214" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A214" s="4" t="s">
+      <c r="A214" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="B214" s="4" t="s">
+      <c r="B214" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="C214" s="4"/>
-      <c r="D214" s="4" t="s">
+      <c r="C214" s="3"/>
+      <c r="D214" s="3" t="s">
         <v>231</v>
       </c>
       <c r="E214">
@@ -21430,14 +21342,14 @@
       </c>
     </row>
     <row r="215" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A215" s="4" t="s">
+      <c r="A215" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="B215" s="4" t="s">
+      <c r="B215" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="C215" s="4"/>
-      <c r="D215" s="4" t="s">
+      <c r="C215" s="3"/>
+      <c r="D215" s="3" t="s">
         <v>229</v>
       </c>
       <c r="E215">
@@ -21523,14 +21435,14 @@
       </c>
     </row>
     <row r="216" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A216" s="4" t="s">
+      <c r="A216" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="B216" s="4" t="s">
+      <c r="B216" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="C216" s="4"/>
-      <c r="D216" s="4" t="s">
+      <c r="C216" s="3"/>
+      <c r="D216" s="3" t="s">
         <v>177</v>
       </c>
       <c r="E216">
@@ -21616,14 +21528,14 @@
       </c>
     </row>
     <row r="217" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A217" s="4" t="s">
+      <c r="A217" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="B217" s="4" t="s">
+      <c r="B217" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="C217" s="4"/>
-      <c r="D217" s="4" t="s">
+      <c r="C217" s="3"/>
+      <c r="D217" s="3" t="s">
         <v>235</v>
       </c>
       <c r="E217">
@@ -21709,14 +21621,14 @@
       </c>
     </row>
     <row r="218" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A218" s="4" t="s">
+      <c r="A218" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="B218" s="4" t="s">
+      <c r="B218" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="C218" s="4"/>
-      <c r="D218" s="4" t="s">
+      <c r="C218" s="3"/>
+      <c r="D218" s="3" t="s">
         <v>231</v>
       </c>
       <c r="E218">
@@ -21802,14 +21714,14 @@
       </c>
     </row>
     <row r="219" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A219" s="4" t="s">
+      <c r="A219" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="B219" s="4" t="s">
+      <c r="B219" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="C219" s="4"/>
-      <c r="D219" s="4" t="s">
+      <c r="C219" s="3"/>
+      <c r="D219" s="3" t="s">
         <v>237</v>
       </c>
       <c r="E219">
@@ -21895,14 +21807,14 @@
       </c>
     </row>
     <row r="220" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A220" s="4" t="s">
+      <c r="A220" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="B220" s="4" t="s">
+      <c r="B220" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="C220" s="4"/>
-      <c r="D220" s="4" t="s">
+      <c r="C220" s="3"/>
+      <c r="D220" s="3" t="s">
         <v>178</v>
       </c>
       <c r="E220">
@@ -22000,123 +21912,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C67B0F93-FA90-0647-BF2D-08F4C72CFDCB}">
-  <sheetPr>
-    <tabColor rgb="FF92D050"/>
-  </sheetPr>
-  <dimension ref="A1:A19"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="86.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A2" s="6" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A3" s="6" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A4" s="6" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A5" s="6" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A6" s="6" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A7" s="6" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A8" s="6" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A9" s="6" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A10" s="6" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A11" s="6" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A12" s="6" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A13" s="6" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A14" s="6" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A15" s="6" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A16" s="6" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A17" s="6" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A18" s="6" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A19" s="6" t="s">
-        <v>263</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>